<commit_message>
Update presentase fuzzy matching.xlsx
</commit_message>
<xml_diff>
--- a/Fuzzy Matching/presentase fuzzy matching.xlsx
+++ b/Fuzzy Matching/presentase fuzzy matching.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{860D3C2B-2F47-471B-998C-0CFA24E5812D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1513081C-7923-4F07-9B81-D0D2DB4CB88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,7 +587,7 @@
       </c>
       <c r="F3">
         <f>((B14-B29)/B29)*100</f>
-        <v>-0.944433908590946</v>
+        <v>5.9169353309311523</v>
       </c>
       <c r="G3">
         <f>((C14-C29)/C29)*100</f>
@@ -701,7 +701,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4">
-        <v>0.39700000000000002</v>
+        <v>0.93969999999999998</v>
       </c>
       <c r="C10" s="4">
         <v>0.996</v>
@@ -753,7 +753,7 @@
       </c>
       <c r="B14" s="6">
         <f>SUM(B3:B12)/10</f>
-        <v>0.78347999999999995</v>
+        <v>0.83774999999999999</v>
       </c>
       <c r="C14" s="6">
         <f>SUM(C3:C12)/10</f>

</xml_diff>